<commit_message>
fix: <aside> páginas de publicaciones
</commit_message>
<xml_diff>
--- a/src/Faltantes.xlsx
+++ b/src/Faltantes.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Contenido Técnico Faltante: Git Tag</t>
   </si>
@@ -104,18 +104,6 @@
   </si>
   <si>
     <t>Aspectos Prácticos Faltantes:</t>
-  </si>
-  <si>
-    <t>5. Casos de error comunes</t>
-  </si>
-  <si>
-    <t>Qué hacer si se crea un tag con el nombre incorrecto</t>
-  </si>
-  <si>
-    <t>Problemas de sincronización entre repositorio local y remoto</t>
-  </si>
-  <si>
-    <t>Conflictos al hacer push de tags</t>
   </si>
   <si>
     <t>6. Estrategias de versionado:</t>
@@ -1120,10 +1108,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A44"/>
+  <dimension ref="A1:A38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="13.8"/>
@@ -1253,26 +1241,6 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
-      <c r="A40" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1">
-      <c r="A44" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>